<commit_message>
mis a jour fct verification des donnees
</commit_message>
<xml_diff>
--- a/GDP/fonction verification données.xlsx
+++ b/GDP/fonction verification données.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamza/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamza/project-grp24/GDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1172407-5059-9242-BFF1-429408DBED94}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD4FD35-1292-F649-87B1-E8F32702CE50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{17B5743F-38DD-5A47-AA32-8F10570FB4D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Liste des fonctions pour vérifier les données</t>
   </si>
@@ -51,85 +51,114 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Tous les candidat en MP sont-ils MP_SPE</t>
-  </si>
-  <si>
-    <t>Pareil en PSI</t>
-  </si>
-  <si>
-    <t>Tous les admis sont-ils admissibles en MP</t>
-  </si>
-  <si>
-    <t>Pareil en PC</t>
-  </si>
-  <si>
-    <t>Pareil en PT</t>
-  </si>
-  <si>
-    <t>Pareil en TSI</t>
-  </si>
-  <si>
-    <t>ADMIS_MP.xlsx
-ADMISSIBLE_MP.xlsx
-ADMIS_MP-SPE.xlsx
-ADMISSIBLE_MP-SPE.xlsx</t>
-  </si>
-  <si>
-    <t>ADMIS_PSI.xlsx
-ADMISSIBLE_PSI.xlsx
-ADMIS_PSI-SPE.xlsx
-ADMISSIBLE_PSI-SPE.xlsx</t>
-  </si>
-  <si>
-    <t>ADMIS_PC.xlsx
-ADMISSIBLE_PC.xlsx
-ADMIS_PC-SPE.xlsx
-ADMISSIBLE_PC-SPE.xlsx</t>
-  </si>
-  <si>
-    <t>ADMIS_PT.xlsx
-ADMISSIBLE_PT.xlsx
-ADMIS_PT-SPE.xlsx
-ADMISSIBLE_PT-SPE.xlsx</t>
-  </si>
-  <si>
-    <t>ADMIS_TSI.xlsx
-ADMISSIBLE_TSI.xlsx
-ADMIS_TSI-SPE.xlsx
-ADMISSIBLE_TSI-SPE.xlsx</t>
-  </si>
-  <si>
-    <t>Pareil en ATS</t>
-  </si>
-  <si>
-    <t>ADMIS_ATS.xlsx
-ADMISSIBLE_ATS.xlsx</t>
-  </si>
-  <si>
-    <t>Verification de l'unicité des id des candidats</t>
-  </si>
-  <si>
     <t>Lecture des fichiers xlxs/csv en python</t>
   </si>
   <si>
-    <t>Le lien entre type admissible (fichier Classe) et candidat spe ou non spé</t>
-  </si>
-  <si>
-    <t>Classes_MP_CMT_spe_XXXX.xlsx
-Classes_PSI_CMT_spe_XXXX.xlsx
-Classes_PC_CMT_spe_XXXX.xlsx
-Classes_PT_CMT_spe_XXXX.xlsx
-…</t>
-  </si>
-  <si>
-    <t>Verifier si les deux colonnes bonification sont les même</t>
+    <t>fichiers ADMIS/ADMISSIBLE</t>
+  </si>
+  <si>
+    <t>admis_admissible.py</t>
+  </si>
+  <si>
+    <t>verifie que tous les élèves admis sont bien admissible</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>classeSPE.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chercher le lien entre les candidat admis/admissible en normal et les candidat admis/admissible en spé </t>
+  </si>
+  <si>
+    <t>Tous les admis sont-ils admissibles</t>
+  </si>
+  <si>
+    <t>Tous les candidats en normal sont-ils en spé ?</t>
+  </si>
+  <si>
+    <t>idunique.py</t>
+  </si>
+  <si>
+    <t>fichiers_admis
+fichiers_CMT
+fichiers_Classes_xlsx
+fichiers_Classes_csv
+fichiers_Ecrit
+fichiers_Oral
+Inscription.xlsx/ResultatEcrit_DD_MM_YYYY_ATS.xlsx/ResultatOral_DD_MM_YYYY_ATS.xlsx/listeEcoles.xlsx/listeEtablissements.xlsx/listeEtatsReponsesAppel.xlsx</t>
+  </si>
+  <si>
+    <t>Verification de l'unicité des id des fhichiers</t>
+  </si>
+  <si>
+    <t>Reponse / Remarque</t>
+  </si>
+  <si>
+    <t>Dans listeEtablissement, certains id se repètent et n'indiquent pas le même établissement</t>
+  </si>
+  <si>
+    <t>fichiers_Classes_xlsx</t>
+  </si>
+  <si>
+    <t>bonification.py</t>
+  </si>
+  <si>
+    <t>verifie que les bonifications ecrites et orales sont les mêmes</t>
+  </si>
+  <si>
+    <t>Les bonifications sont-elles les mêmes ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chercher le lien entre le type_admissible et les candidat admis/admissibles en spé </t>
+  </si>
+  <si>
+    <t>Les type admissible A sont les élèves ADMIS en normale Les type admissible B sont les élèves ADMIS en spé seulement
+Les fichiers_classes ne concernent que les candidats admis.</t>
+  </si>
+  <si>
+    <t>typeadmissible.py</t>
+  </si>
+  <si>
+    <t>fichiers ADMIS/ADMISSIBLE
+fichiers_Classes_xlsx</t>
+  </si>
+  <si>
+    <t>ecritutre_file.py</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Ecrit un fichier txt avec tous les fichiers de data et leurs colonnes.</t>
+  </si>
+  <si>
+    <t>Ce fichier permettra d'avoir acces rapidement aux colonnes des donnees et d'inserer à côté des colonnes les champs correspondant dans la base de donnee</t>
+  </si>
+  <si>
+    <t>compare.py</t>
+  </si>
+  <si>
+    <t>la fonction compare permet de comparer deux colonnes dans deux fichiers à partir des colonnes clés à partir de deux triplet.
+On peut par exemple comparer les rang des candidats dans Classes_MP_CMT_spe_XXXX.xlsx et dans Oral_MP.xlsx ainsi :
+compare( ('Classes_MP_CMT_spe_XXXX.xlsx' , 'login' , 'rang_classe') , ('Oral_MP.xlsx' , 'Can _cod' , 'rang') )</t>
+  </si>
+  <si>
+    <t>La fonction ne compare que les valeurs des clés presentes dans les deux tables. Elle ne precisera pas que certaines clés sont manquantes dans une table</t>
+  </si>
+  <si>
+    <t>contient.py</t>
+  </si>
+  <si>
+    <t>Lafonction contient( (fichier1, colonne1) , (fichier2,colonne2) ) renvoie vrai si colonne1 contient tous les elements de colonne2 et faux sinon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,6 +171,13 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri (Corps)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,11 +200,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -489,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140BFA75-803F-F046-B82E-C5BF49591F5C}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,32 +540,33 @@
     <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="33.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="38" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -540,132 +581,148 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="44" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="44" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:18" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>14</v>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="E22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>